<commit_message>
Avance en la carga del set_up
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorización\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B5777-3E6D-4E0C-A4FA-596FDD34D343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -12,14 +18,13 @@
     <sheet name="OrdenEstandar" sheetId="3" r:id="rId3"/>
     <sheet name="Maquinas" sheetId="4" r:id="rId4"/>
     <sheet name="ReglasCambio" sheetId="5" r:id="rId5"/>
-    <sheet name="Responsables" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Parametro</t>
   </si>
@@ -57,9 +62,6 @@
     <t>Impresión</t>
   </si>
   <si>
-    <t>Enchapado</t>
-  </si>
-  <si>
     <t>OPP</t>
   </si>
   <si>
@@ -96,9 +98,6 @@
     <t>Manual 1</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
     <t>Ventanas</t>
   </si>
   <si>
@@ -114,9 +113,6 @@
     <t>Descartonadora</t>
   </si>
   <si>
-    <t>Enchapadora</t>
-  </si>
-  <si>
     <t>Ideal para tiradas largas</t>
   </si>
   <si>
@@ -159,38 +155,29 @@
     <t>Misma medida de pliego/arte</t>
   </si>
   <si>
-    <t>Responsable</t>
-  </si>
-  <si>
-    <t>Operario A</t>
-  </si>
-  <si>
-    <t>Operario B</t>
-  </si>
-  <si>
-    <t>Tercerizado</t>
-  </si>
-  <si>
-    <t>Operario C</t>
-  </si>
-  <si>
-    <t>Operario D</t>
-  </si>
-  <si>
-    <t>Operario E</t>
-  </si>
-  <si>
-    <t>Operario F</t>
-  </si>
-  <si>
-    <t>Operario G</t>
+    <t>Barniz</t>
+  </si>
+  <si>
+    <t>Stamping</t>
+  </si>
+  <si>
+    <t>Cuño</t>
+  </si>
+  <si>
+    <t>Encapado</t>
+  </si>
+  <si>
+    <t>Encapadora</t>
+  </si>
+  <si>
+    <t>Manual 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,24 +229,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -297,7 +293,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -331,6 +327,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -365,9 +362,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,14 +538,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -563,7 +566,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -571,12 +574,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -586,18 +590,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -608,14 +613,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -623,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -631,7 +638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -639,52 +646,76 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -693,39 +724,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -737,15 +777,15 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>1000</v>
@@ -757,32 +797,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
         <v>4000</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>1200</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -791,12 +831,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>1500</v>
@@ -808,12 +848,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>6000</v>
@@ -825,15 +865,15 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>7000</v>
@@ -845,15 +885,15 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>9000</v>
@@ -865,12 +905,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>3000</v>
@@ -882,12 +922,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>3500</v>
@@ -899,12 +939,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>2800</v>
@@ -922,151 +962,73 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrega proceso de impresion priorizado, falta pegado-ventana
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorización\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B5777-3E6D-4E0C-A4FA-596FDD34D343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B35FF7-C3B6-441C-9BAA-4D346FEF7129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Parametro</t>
   </si>
@@ -80,97 +80,106 @@
     <t>Maquina</t>
   </si>
   <si>
+    <t>Setup_base_min</t>
+  </si>
+  <si>
+    <t>Setup_menor_min</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Automática</t>
+  </si>
+  <si>
+    <t>Manual 1</t>
+  </si>
+  <si>
+    <t>Ventanas</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Flexo</t>
+  </si>
+  <si>
+    <t>Guillotina 1</t>
+  </si>
+  <si>
+    <t>Descartonadora</t>
+  </si>
+  <si>
+    <t>Ideal para tiradas largas</t>
+  </si>
+  <si>
+    <t>Papel/Cartulina</t>
+  </si>
+  <si>
+    <t>Microcorrugado</t>
+  </si>
+  <si>
+    <t>Criterio</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Aplicar_setup_menor</t>
+  </si>
+  <si>
+    <t>Mismo_CodigoTroquel</t>
+  </si>
+  <si>
+    <t>Misma_Marca</t>
+  </si>
+  <si>
+    <t>Mismos_Colores</t>
+  </si>
+  <si>
+    <t>Mismo_Tamano</t>
+  </si>
+  <si>
+    <t>Mantener mismo troquel en troqueladora</t>
+  </si>
+  <si>
+    <t>Misma marca/cliente en impresión</t>
+  </si>
+  <si>
+    <t>Igual combinación CMYK / Pantone</t>
+  </si>
+  <si>
+    <t>Misma medida de pliego/arte</t>
+  </si>
+  <si>
+    <t>Barniz</t>
+  </si>
+  <si>
+    <t>Stamping</t>
+  </si>
+  <si>
+    <t>Cuño</t>
+  </si>
+  <si>
+    <t>Encapado</t>
+  </si>
+  <si>
+    <t>Encapadora</t>
+  </si>
+  <si>
+    <t>Manual 2</t>
+  </si>
+  <si>
     <t>Capacidad_pliegos_hora</t>
   </si>
   <si>
-    <t>Setup_base_min</t>
-  </si>
-  <si>
-    <t>Setup_menor_min</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t>Automática</t>
-  </si>
-  <si>
-    <t>Manual 1</t>
-  </si>
-  <si>
-    <t>Ventanas</t>
-  </si>
-  <si>
-    <t>Offset</t>
-  </si>
-  <si>
-    <t>Flexo</t>
-  </si>
-  <si>
-    <t>Guillotina 1</t>
-  </si>
-  <si>
-    <t>Descartonadora</t>
-  </si>
-  <si>
-    <t>Ideal para tiradas largas</t>
-  </si>
-  <si>
-    <t>Papel/Cartulina</t>
-  </si>
-  <si>
-    <t>Microcorrugado</t>
-  </si>
-  <si>
-    <t>Criterio</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Aplicar_setup_menor</t>
-  </si>
-  <si>
-    <t>Mismo_CodigoTroquel</t>
-  </si>
-  <si>
-    <t>Misma_Marca</t>
-  </si>
-  <si>
-    <t>Mismos_Colores</t>
-  </si>
-  <si>
-    <t>Mismo_Tamano</t>
-  </si>
-  <si>
-    <t>Mantener mismo troquel en troqueladora</t>
-  </si>
-  <si>
-    <t>Misma marca/cliente en impresión</t>
-  </si>
-  <si>
-    <t>Igual combinación CMYK / Pantone</t>
-  </si>
-  <si>
-    <t>Misma medida de pliego/arte</t>
-  </si>
-  <si>
-    <t>Barniz</t>
-  </si>
-  <si>
-    <t>Stamping</t>
-  </si>
-  <si>
-    <t>Cuño</t>
-  </si>
-  <si>
-    <t>Encapado</t>
-  </si>
-  <si>
-    <t>Encapadora</t>
-  </si>
-  <si>
-    <t>Manual 2</t>
+    <t>Impresión Offset</t>
+  </si>
+  <si>
+    <t>Impresión Flexo</t>
+  </si>
+  <si>
+    <t>Pegadora 1</t>
   </si>
 </sst>
 </file>
@@ -229,12 +238,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +586,6 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -651,7 +658,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -675,7 +682,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -683,7 +690,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -727,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,16 +755,16 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -765,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -777,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,7 +792,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>1000</v>
@@ -802,7 +809,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>1000</v>
@@ -819,7 +826,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>4000</v>
@@ -836,7 +843,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>1500</v>
@@ -850,10 +857,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>6000</v>
@@ -865,15 +872,15 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>7000</v>
@@ -885,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>9000</v>
@@ -910,7 +917,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>3000</v>
@@ -941,10 +948,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
       </c>
       <c r="C12">
         <v>2800</v>
@@ -978,21 +985,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1000,10 +1007,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1011,10 +1018,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1022,10 +1029,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Solucionado el orden de procesos
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorización\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F83750C-94FF-4B29-B9FD-93087AE0374F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B6EA97-1F95-463B-8CE0-E4C1A97DB4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Parametro</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Guillotina</t>
   </si>
   <si>
-    <t>Impresión</t>
-  </si>
-  <si>
     <t>Barniz</t>
   </si>
   <si>
@@ -109,12 +106,6 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>Automática</t>
-  </si>
-  <si>
-    <t>Ideal para tiradas largas</t>
-  </si>
-  <si>
     <t>Manual 1</t>
   </si>
   <si>
@@ -133,18 +124,12 @@
     <t>Offset</t>
   </si>
   <si>
-    <t>Papel/Cartulina</t>
-  </si>
-  <si>
     <t>Impresión Flexo</t>
   </si>
   <si>
     <t>Flexo</t>
   </si>
   <si>
-    <t>Microcorrugado</t>
-  </si>
-  <si>
     <t>Guillotina 1</t>
   </si>
   <si>
@@ -157,12 +142,6 @@
     <t>Barnizado</t>
   </si>
   <si>
-    <t>DescartonadoraM1</t>
-  </si>
-  <si>
-    <t>DescartonadoraM2</t>
-  </si>
-  <si>
     <t>Manual1/Manual2</t>
   </si>
   <si>
@@ -197,13 +176,16 @@
   </si>
   <si>
     <t>Misma medida de pliego/arte</t>
+  </si>
+  <si>
+    <t>Automatica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,14 +195,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -268,8 +242,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -575,79 +551,87 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>20</v>
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -658,10 +642,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,6 +655,7 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -678,369 +663,266 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+        <v>5</v>
+      </c>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="D4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
       <c r="C5">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>1500</v>
+        <v>3500</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E7">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
       <c r="C8">
-        <v>3000</v>
+        <v>2800</v>
       </c>
       <c r="D8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>5000</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9">
-        <v>9000</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>7</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C11">
-        <v>3500</v>
+        <v>1000</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>2800</v>
+        <v>3000</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="D13">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C14">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C15">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16">
-        <v>1000</v>
-      </c>
-      <c r="D16">
-        <v>25</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="C16" s="2"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <dataValidations count="1">
+    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="B6 H6" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1067,21 +949,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1089,10 +971,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1100,10 +982,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1111,10 +993,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Solucion de orden de procesos y se agregan descartonadoras
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorización\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B6EA97-1F95-463B-8CE0-E4C1A97DB4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4951CEEF-3D11-4B0E-9607-7452E0290420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Parametro</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Guillotina 1</t>
   </si>
   <si>
-    <t>Descartonadora</t>
-  </si>
-  <si>
     <t>Encapadora</t>
   </si>
   <si>
@@ -179,6 +176,12 @@
   </si>
   <si>
     <t>Automatica</t>
+  </si>
+  <si>
+    <t>Descartonadora 1</t>
+  </si>
+  <si>
+    <t>Descartonadora 2</t>
   </si>
 </sst>
 </file>
@@ -237,13 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -558,7 +560,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -642,10 +644,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,7 +696,7 @@
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="M2" s="3"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -732,7 +734,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -769,7 +771,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>1000</v>
@@ -786,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>2800</v>
@@ -803,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9">
         <v>5000</v>
@@ -854,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>3000</v>
@@ -871,7 +873,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>3000</v>
@@ -916,9 +918,6 @@
       <c r="E15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -949,21 +948,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -971,10 +970,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -982,10 +981,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -993,10 +992,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Gannt corregido por dia, falta por semana y por mes
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorización\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B7E2BC-817F-4B97-98EC-7994D3A61484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F17E9A-14E0-4CAB-8D97-82121174B4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -284,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -293,6 +293,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" activeCellId="1" sqref="C18:C19 E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -513,14 +514,14 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>8.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -692,7 +693,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -980,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DBCE81-1EC7-4DD7-8152-594C97F4CF66}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambio de clave de priorizacion en offset
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t xml:space="preserve">Parametro</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve">Descartonadora 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descartonadora 3</t>
   </si>
   <si>
     <t xml:space="preserve">Ventanas</t>
@@ -745,7 +748,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -804,13 +807,13 @@
         <v>28</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>5000</v>
+        <v>3500</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,10 +824,10 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>3000</v>
+        <v>1100</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>12</v>
@@ -855,7 +858,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>30</v>
@@ -872,13 +875,13 @@
         <v>32</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,13 +892,13 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,13 +909,13 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,24 +954,24 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>38</v>
@@ -977,13 +980,29 @@
         <v>1500</v>
       </c>
       <c r="D13" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E14" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1014,15 +1033,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -1030,7 +1049,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -1038,7 +1057,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -1046,7 +1065,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -1054,7 +1073,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1062,7 +1081,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
@@ -1070,7 +1089,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -1078,7 +1097,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>30</v>
@@ -1086,7 +1105,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1094,7 +1113,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -1131,21 +1150,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -1153,10 +1172,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1164,10 +1183,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -1175,10 +1194,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Agrega solucion al cambio de orden entre impresion offset y barnizado
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t xml:space="preserve">Parametro</t>
   </si>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Impresión Offset</t>
   </si>
   <si>
-    <t xml:space="preserve">Barniz</t>
+    <t xml:space="preserve">Barnizado</t>
   </si>
   <si>
     <t xml:space="preserve">OPP</t>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t xml:space="preserve">Flexo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barnizado</t>
   </si>
   <si>
     <t xml:space="preserve">Automatica</t>
@@ -616,8 +613,8 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,8 +744,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -835,7 +832,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>
@@ -855,7 +852,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>4000</v>
@@ -872,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>750</v>
@@ -889,7 +886,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>750</v>
@@ -906,7 +903,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>750</v>
@@ -923,7 +920,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>3000</v>
@@ -940,7 +937,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>3000</v>
@@ -957,7 +954,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>3000</v>
@@ -974,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1500</v>
@@ -991,7 +988,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>4000</v>
@@ -1033,15 +1030,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -1049,7 +1046,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -1057,7 +1054,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -1065,7 +1062,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -1073,7 +1070,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1081,7 +1078,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
@@ -1089,7 +1086,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -1097,15 +1094,15 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1113,7 +1110,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -1150,21 +1147,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -1172,10 +1169,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1183,10 +1180,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -1194,10 +1191,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Agrega planificacion con plastificado
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorizacion_theiler\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D93FE1F-4E2A-460A-8ED9-53D3740E7D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B91C948-7AB2-4065-BF09-BF265F316C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>Parametro</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Plastificado</t>
+  </si>
+  <si>
+    <t>Plastificadora</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -688,10 +691,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -795,16 +798,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C6">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -815,16 +818,16 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>750</v>
+        <v>4000</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -832,7 +835,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>750</v>
@@ -849,7 +852,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>750</v>
@@ -863,27 +866,27 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10">
-        <v>3000</v>
+        <v>750</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>3000</v>
@@ -900,7 +903,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>3000</v>
@@ -914,39 +917,55 @@
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>1500</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>4000</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>20</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>8</v>
       </c>
     </row>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Agrega proceso de encapado y stamping
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorizacion_theiler\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B91C948-7AB2-4065-BF09-BF265F316C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512878EF-058C-429C-A9B6-0967F652223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Abreviaturas" sheetId="5" r:id="rId5"/>
     <sheet name="ReglasCambio" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Parametro</t>
   </si>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -691,10 +691,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -798,10 +798,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>1000</v>
@@ -815,16 +815,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C7">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -832,19 +832,19 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="D8">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -852,16 +852,16 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>750</v>
+        <v>4000</v>
       </c>
       <c r="D9">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -869,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>750</v>
@@ -883,44 +883,44 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11">
-        <v>3000</v>
+        <v>750</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12">
-        <v>3000</v>
+        <v>750</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>3000</v>
@@ -934,35 +934,69 @@
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>3000</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>1500</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>4000</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>20</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agrega proceso tercierizado de cuño
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorizacion_theiler\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512878EF-058C-429C-A9B6-0967F652223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F99BDF-3097-4677-A8CF-DA1016F83771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Parametro</t>
   </si>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -691,10 +691,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -849,16 +849,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -869,16 +869,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>750</v>
+        <v>4000</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E10">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -886,7 +886,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>750</v>
@@ -903,7 +903,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>750</v>
@@ -917,27 +917,27 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13">
-        <v>3000</v>
+        <v>750</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>3000</v>
@@ -954,7 +954,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>3000</v>
@@ -968,35 +968,52 @@
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>4000</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>20</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agrega maquina troqueladora iberica
</commit_message>
<xml_diff>
--- a/config/Config_Priorizacion_Theiler.xlsx
+++ b/config/Config_Priorizacion_Theiler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Fran\Trabajo\Theiler\proyecto_priorizacion_theiler\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CABDFAE-EFFD-4E63-802B-578481BA3733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898E59BB-9657-4CB9-871B-CDF14D7A78AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornada" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Parametro</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Bobina</t>
+  </si>
+  <si>
+    <t>Iberica</t>
   </si>
 </sst>
 </file>
@@ -308,13 +311,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -727,10 +730,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -740,6 +743,7 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -988,27 +992,27 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C15">
-        <v>3000</v>
+        <v>2600</v>
       </c>
       <c r="D15">
+        <v>45</v>
+      </c>
+      <c r="E15">
         <v>15</v>
       </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>3000</v>
@@ -1025,7 +1029,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>3000</v>
@@ -1039,35 +1043,52 @@
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E18">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>1500</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>4000</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>20</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>8</v>
       </c>
     </row>
@@ -1188,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>